<commit_message>
document tests to be done
</commit_message>
<xml_diff>
--- a/Doc/Test/Ejemplo test.xlsx
+++ b/Doc/Test/Ejemplo test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/didacrius/Desktop/LaSalle Gracia/TicTacToe/TestTicTacToe/Doc/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BAE6413-624D-4155-A0D9-2D5A9C86F920}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B16CE8-E66D-8748-AF34-E409471B428D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11209586-37A8-46D7-A8FA-E22058FA9608}"/>
+    <workbookView xWindow="11280" yWindow="0" windowWidth="17520" windowHeight="18000" xr2:uid="{11209586-37A8-46D7-A8FA-E22058FA9608}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,32 +31,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="36">
   <si>
     <t>Resultats reals</t>
   </si>
   <si>
-    <t>Nom prova</t>
-  </si>
-  <si>
     <t>Objectiu prova</t>
   </si>
   <si>
     <t>Valors d'entrada</t>
   </si>
   <si>
-    <t>Aquesta prova servira …</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
     <t>Valor</t>
   </si>
   <si>
-    <t>Nom variable</t>
-  </si>
-  <si>
     <t>Resultat esperats</t>
   </si>
   <si>
@@ -70,13 +61,91 @@
   </si>
   <si>
     <t>Nom variable sortida</t>
+  </si>
+  <si>
+    <t>BoardIsCreatedSuccessfully</t>
+  </si>
+  <si>
+    <t>Board se instancia correctmente.</t>
+  </si>
+  <si>
+    <t>players</t>
+  </si>
+  <si>
+    <t>player1, player2</t>
+  </si>
+  <si>
+    <t>squares</t>
+  </si>
+  <si>
+    <t>square1…square16</t>
+  </si>
+  <si>
+    <t>board</t>
+  </si>
+  <si>
+    <t>empty square values</t>
+  </si>
+  <si>
+    <t>El método move se realiza correctamente seteando un su símbolo en una posición.</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>player's symbol</t>
+  </si>
+  <si>
+    <t>square position</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>WhenPlayerMovesToAPositionWhichIsEmptyHisSymbolIsSetIntoASquare</t>
+  </si>
+  <si>
+    <t>WhenPlayerMovesToAPositionWhichIsNotEmptyHisSymbolIsNotSetIntoASquare</t>
+  </si>
+  <si>
+    <t>isFullReturnsTrueWhenAllSquaresAreFull</t>
+  </si>
+  <si>
+    <t>El método isFull comprueba correctamente que todas las casillas estén ocupadas devolviendo true.</t>
+  </si>
+  <si>
+    <t>isFullReturnsTrueWhenAllSquaresAreNotFull</t>
+  </si>
+  <si>
+    <t>El método isFull comprueba correctamente que todas las casillas no estén ocupadas devolviendo false.</t>
+  </si>
+  <si>
+    <t>GivenAPlayerTurnWhenNextTurnIsCalledTheTurnChangesToAnotherPlayer</t>
+  </si>
+  <si>
+    <t>El método next turn cambia el turno al siguiente jugador.</t>
+  </si>
+  <si>
+    <t>turn</t>
+  </si>
+  <si>
+    <t>GivenAPlayerTurnWhenNextTurnIsCalledUntilSamePlayerReceivesTheTurnTheTurnIsTheSameAsInTheStart</t>
+  </si>
+  <si>
+    <t>0 (el mismo que empieza)</t>
+  </si>
+  <si>
+    <t>WhenATurnIsFinishedAnd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +153,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,8 +204,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF81B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF2D2D"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -249,72 +361,208 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -342,7 +590,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -638,115 +886,727 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E30E8BB-7E5A-487F-ACE6-81D7E5408359}">
-  <dimension ref="C4:D17"/>
+  <dimension ref="C4:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B88" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
+    <row r="4" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="3:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="7" t="s">
+      <c r="D20" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C28" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="9" t="s">
+      <c r="D28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="10" t="s">
+    </row>
+    <row r="29" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="20"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C43" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C12" s="11" t="s">
+      <c r="D43" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="16"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="20"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="13" t="s">
+      <c r="D56" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="22"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C14" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="17" t="s">
+      <c r="D59" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C62" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" s="16"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C64" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="18"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="5"/>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C67" s="5"/>
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C68" s="5"/>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C69" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="20"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C70" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="19" t="s">
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C72" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="22"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="D74" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C77" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" s="38"/>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C79" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="40"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C80" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C81" s="27"/>
+      <c r="D81" s="28"/>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C82" s="27"/>
+      <c r="D82" s="28"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C83" s="27"/>
+      <c r="D83" s="28"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C84" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="42"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C85" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C86" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C87" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="44"/>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C88" s="33" t="s">
         <v>6</v>
       </c>
+      <c r="D88" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C92" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" s="38"/>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C93" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C94" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="40"/>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C95" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C96" s="27"/>
+      <c r="D96" s="28"/>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C97" s="27"/>
+      <c r="D97" s="28"/>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C98" s="27"/>
+      <c r="D98" s="28"/>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C99" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="42"/>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C100" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C101" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C102" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="44"/>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C103" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" s="36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C107" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D107" s="38"/>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C108" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C109" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" s="40"/>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C110" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C111" s="27"/>
+      <c r="D111" s="28"/>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C112" s="27"/>
+      <c r="D112" s="28"/>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C113" s="27"/>
+      <c r="D113" s="28"/>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C114" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="42"/>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C115" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D115" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C116" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C117" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D117" s="44"/>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C118" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C119" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" s="36" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="31">
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>